<commit_message>
modify add sub tableview
</commit_message>
<xml_diff>
--- a/Config/partsParam.xlsx
+++ b/Config/partsParam.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -26,10 +26,19 @@
     <t>Unit</t>
   </si>
   <si>
+    <t>MultChoose</t>
+  </si>
+  <si>
     <t>Force</t>
   </si>
   <si>
-    <t>subForm</t>
+    <t>SubForm</t>
+  </si>
+  <si>
+    <t>AdditionalForm</t>
+  </si>
+  <si>
+    <t>AdditionalValue</t>
   </si>
   <si>
     <t>零件号</t>
@@ -44,7 +53,13 @@
     <t>2</t>
   </si>
   <si>
-    <t>packageDetail</t>
+    <t>packageType</t>
+  </si>
+  <si>
+    <t>additional</t>
+  </si>
+  <si>
+    <t>[3,4,5,6]</t>
   </si>
   <si>
     <t>零件长</t>
@@ -63,6 +78,9 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>[0,1,2]</t>
   </si>
   <si>
     <t>包装模数</t>
@@ -108,7 +126,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -121,6 +139,11 @@
     </font>
     <font>
       <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
@@ -162,7 +185,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -209,6 +232,21 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="11"/>
       </left>
       <right style="thin">
@@ -318,53 +356,56 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1485,11 +1526,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="12" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="16.3516" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.3516" style="1" customWidth="1"/>
@@ -1498,7 +1539,9 @@
     <col min="5" max="5" width="16.3516" style="1" customWidth="1"/>
     <col min="6" max="6" width="16.3516" style="1" customWidth="1"/>
     <col min="7" max="7" width="16.3516" style="1" customWidth="1"/>
-    <col min="8" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.3516" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.3516" style="1" customWidth="1"/>
+    <col min="10" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="31" customHeight="1">
@@ -1506,305 +1549,367 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="E1" s="4"/>
       <c r="F1" s="3"/>
-      <c r="G1" s="4"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="6"/>
     </row>
     <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" t="s" s="5">
+      <c r="A2" t="s" s="7">
         <v>0</v>
       </c>
-      <c r="B2" t="s" s="5">
+      <c r="B2" t="s" s="7">
         <v>1</v>
       </c>
-      <c r="C2" t="s" s="5">
+      <c r="C2" t="s" s="7">
         <v>2</v>
       </c>
-      <c r="D2" t="s" s="5">
+      <c r="D2" t="s" s="7">
         <v>3</v>
       </c>
-      <c r="E2" t="s" s="5">
+      <c r="E2" t="s" s="7">
         <v>4</v>
       </c>
-      <c r="F2" t="s" s="5">
+      <c r="F2" t="s" s="7">
         <v>5</v>
       </c>
-      <c r="G2" s="6"/>
+      <c r="G2" t="s" s="7">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s" s="7">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" ht="24.55" customHeight="1">
-      <c r="A3" s="7">
+      <c r="A3" s="8">
         <v>0</v>
       </c>
-      <c r="B3" t="s" s="8">
+      <c r="B3" t="s" s="9">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s" s="10">
+        <v>10</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" ht="24.35" customHeight="1">
+      <c r="A4" s="12">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s" s="14">
+        <v>12</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" t="s" s="14">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s" s="14">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s" s="14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" ht="24.35" customHeight="1">
+      <c r="A5" s="12">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s" s="13">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s" s="14">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s" s="14">
+        <v>17</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+    </row>
+    <row r="6" ht="24.35" customHeight="1">
+      <c r="A6" s="12">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s" s="13">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s" s="14">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s" s="14">
+        <v>17</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+    </row>
+    <row r="7" ht="24.35" customHeight="1">
+      <c r="A7" s="12">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s" s="13">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s" s="14">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s" s="14">
+        <v>17</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+    </row>
+    <row r="8" ht="24.35" customHeight="1">
+      <c r="A8" s="12">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s" s="13">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s" s="14">
+        <v>21</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="14"/>
+      <c r="H8" t="s" s="14">
+        <v>14</v>
+      </c>
+      <c r="I8" t="s" s="14">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" ht="24.35" customHeight="1">
+      <c r="A9" s="12">
         <v>6</v>
       </c>
-      <c r="C3" t="s" s="9">
+      <c r="B9" t="s" s="13">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s" s="14">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s" s="14">
+        <v>24</v>
+      </c>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+    </row>
+    <row r="10" ht="24.35" customHeight="1">
+      <c r="A10" s="12">
         <v>7</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-    </row>
-    <row r="4" ht="24.35" customHeight="1">
-      <c r="A4" s="11">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s" s="12">
+      <c r="B10" t="s" s="13">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s" s="14">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s" s="14">
+        <v>26</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+    </row>
+    <row r="11" ht="24.35" customHeight="1">
+      <c r="A11" s="12">
         <v>8</v>
       </c>
-      <c r="C4" t="s" s="13">
+      <c r="B11" t="s" s="13">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s" s="14">
+        <v>28</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" t="s" s="14">
+        <v>29</v>
+      </c>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+    </row>
+    <row r="12" ht="24.35" customHeight="1">
+      <c r="A12" s="12">
         <v>9</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" t="s" s="13">
+      <c r="B12" t="s" s="13">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s" s="14">
+        <v>31</v>
+      </c>
+      <c r="D12" s="15"/>
+      <c r="E12" t="s" s="14">
+        <v>21</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" t="s" s="14">
+        <v>32</v>
+      </c>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+    </row>
+    <row r="13" ht="24.35" customHeight="1">
+      <c r="A13" s="12">
         <v>10</v>
       </c>
-      <c r="G4" s="14"/>
-    </row>
-    <row r="5" ht="24.35" customHeight="1">
-      <c r="A5" s="11">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s" s="12">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s" s="13">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s" s="13">
-        <v>12</v>
-      </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-    </row>
-    <row r="6" ht="24.35" customHeight="1">
-      <c r="A6" s="11">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s" s="12">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s" s="13">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s" s="13">
-        <v>12</v>
-      </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-    </row>
-    <row r="7" ht="24.35" customHeight="1">
-      <c r="A7" s="11">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s" s="12">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s" s="13">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s" s="13">
-        <v>12</v>
-      </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-    </row>
-    <row r="8" ht="24.35" customHeight="1">
-      <c r="A8" s="11">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s" s="13">
-        <v>16</v>
-      </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-    </row>
-    <row r="9" ht="24.35" customHeight="1">
-      <c r="A9" s="11">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s" s="12">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s" s="13">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s" s="13">
-        <v>18</v>
-      </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-    </row>
-    <row r="10" ht="24.35" customHeight="1">
-      <c r="A10" s="11">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s" s="12">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s" s="13">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s" s="13">
-        <v>20</v>
-      </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-    </row>
-    <row r="11" ht="24.35" customHeight="1">
-      <c r="A11" s="11">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s" s="12">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s" s="13">
-        <v>22</v>
-      </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" t="s" s="13">
-        <v>23</v>
-      </c>
-      <c r="G11" s="14"/>
-    </row>
-    <row r="12" ht="24.35" customHeight="1">
-      <c r="A12" s="11">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s" s="12">
-        <v>24</v>
-      </c>
-      <c r="C12" t="s" s="13">
-        <v>25</v>
-      </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" t="s" s="13">
-        <v>26</v>
-      </c>
-      <c r="G12" s="14"/>
-    </row>
-    <row r="13" ht="24.35" customHeight="1">
-      <c r="A13" s="11">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s" s="12">
-        <v>27</v>
-      </c>
-      <c r="C13" t="s" s="13">
-        <v>28</v>
-      </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
+      <c r="B13" t="s" s="13">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s" s="14">
+        <v>34</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
     </row>
     <row r="14" ht="20.35" customHeight="1">
-      <c r="A14" s="11"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
     </row>
     <row r="15" ht="20.35" customHeight="1">
-      <c r="A15" s="11"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
     </row>
     <row r="16" ht="20.35" customHeight="1">
-      <c r="A16" s="11"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
     </row>
     <row r="17" ht="20.35" customHeight="1">
-      <c r="A17" s="11"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
     </row>
     <row r="18" ht="20.35" customHeight="1">
-      <c r="A18" s="11"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
     </row>
     <row r="19" ht="20.35" customHeight="1">
-      <c r="A19" s="11"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
     </row>
     <row r="20" ht="20.35" customHeight="1">
-      <c r="A20" s="11"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
     </row>
     <row r="21" ht="20.35" customHeight="1">
-      <c r="A21" s="11"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
     </row>
     <row r="22" ht="20.35" customHeight="1">
-      <c r="A22" s="11"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
     </row>
     <row r="23" ht="20.35" customHeight="1">
-      <c r="A23" s="11"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>